<commit_message>
Totally refactor to support multiple nested data-row
</commit_message>
<xml_diff>
--- a/assets/sample.xlsx
+++ b/assets/sample.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mine\nextrj\nextrj_xlsx\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F785CB-C54A-47E7-A6D0-A7F802B6ED90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7B82FD-2718-4842-A9D2-2545976ADB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23010" yWindow="8440" windowWidth="15210" windowHeight="12050" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17430" yWindow="1200" windowWidth="20110" windowHeight="16340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="3" r:id="rId1"/>
     <sheet name="with-group" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="v2" guid="{92778668-F09B-4AA4-9177-A44EE1857F73}" xWindow="1631" yWindow="28" windowWidth="2195" windowHeight="1946" activeSheetId="1"/>
     <customWorkbookView name="v1" guid="{971221AF-3C57-49E6-8781-A93ECDACA8CC}" xWindow="1631" yWindow="28" windowWidth="2195" windowHeight="1946" activeSheetId="1"/>
-    <customWorkbookView name="v2" guid="{92778668-F09B-4AA4-9177-A44EE1857F73}" xWindow="1631" yWindow="28" windowWidth="2195" windowHeight="1946" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
   <si>
     <t>Money</t>
   </si>
@@ -156,6 +157,102 @@
   </si>
   <si>
     <t>Simple table example</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[0].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[0].b[0].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[0].b[n].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[‘a', 'k']</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[‘a', 'b', 'k']</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[‘a', 'b', 'c', 'k']</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[0].b[n].c[0].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[0].b[n].c[n].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[n].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[n].b[0].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[n].b[n].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[n].b[0].c[0].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[n].b[0].c[n].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[n].b[n].c[0].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a[n].b[n].c[n].k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>keys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'k'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>without a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a without b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.b without c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.b.c</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -169,7 +266,7 @@
     <numFmt numFmtId="178" formatCode="#0.00"/>
     <numFmt numFmtId="179" formatCode="\￥#,###,###,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +294,15 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +312,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -229,11 +335,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -260,13 +403,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -564,7 +761,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -647,7 +844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E060FA-7C73-4A84-9350-243E4E03117E}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -717,10 +914,10 @@
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
@@ -735,8 +932,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
@@ -751,8 +948,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="1"/>
       <c r="D8" s="5"/>
       <c r="E8" s="1" t="s">
@@ -763,10 +960,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -783,8 +980,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
@@ -799,8 +996,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
@@ -839,4 +1036,227 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BF600C-3439-4025-882A-BB3080BA7152}">
+  <dimension ref="B2:F17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="20" customWidth="1"/>
+    <col min="3" max="3" width="8.58203125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="11.4140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="14"/>
+      <c r="C6" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="F12:F17"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>